<commit_message>
Minor changes in formatting. Linux commit.
</commit_message>
<xml_diff>
--- a/docs/awards.xlsx
+++ b/docs/awards.xlsx
@@ -160,16 +160,20 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -362,123 +366,124 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="68.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="68.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="68.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="68.29"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="C2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="D2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="2"/>
+      <c r="E2" s="3"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="C3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="0" t="s">
+      <c r="D3" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="C4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="0" t="s">
+      <c r="D4" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="0" t="s">
+      <c r="C5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="0" t="s">
+      <c r="D5" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+      <c r="A6" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="0" t="s">
+      <c r="C6" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D6" s="0" t="s">
+      <c r="D6" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+      <c r="A7" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="0" t="s">
+      <c r="C7" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D7" s="0" t="s">
+      <c r="D7" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E7" s="0" t="s">
+      <c r="E7" s="1" t="s">
         <v>20</v>
       </c>
     </row>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>